<commit_message>
fatal: pathspec 'LR3/table_1_73' did not match any files
</commit_message>
<xml_diff>
--- a/LR3/table_1_73.xlsx
+++ b/LR3/table_1_73.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Студент\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE97C774-54B8-424A-8CDF-5D04B8C2D9BD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580" xr2:uid="{29FF570E-F98A-4042-9EB9-0F50A8CD58DC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -150,18 +149,9 @@
     <t>Пени за 1 день</t>
   </si>
   <si>
-    <t>Общая сумма</t>
-  </si>
-  <si>
-    <t>Средняя площадь</t>
-  </si>
-  <si>
     <t>Максимальный срок просрочки</t>
   </si>
   <si>
-    <t>Максимальная сумма</t>
-  </si>
-  <si>
     <t>Площадь, кв.м.</t>
   </si>
   <si>
@@ -178,12 +168,21 @@
   </si>
   <si>
     <t>Итого, руб.</t>
+  </si>
+  <si>
+    <t>Общая сумма, руб.</t>
+  </si>
+  <si>
+    <t>Средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>Максимальная сумма, руб.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -542,17 +541,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73F70FF-5DAE-4603-B700-D2EDE2B4BFDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="2" max="2" width="35.25" customWidth="1"/>
     <col min="3" max="3" width="13.75" customWidth="1"/>
     <col min="4" max="4" width="15.75" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
@@ -577,13 +576,13 @@
         <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>38</v>
@@ -592,16 +591,16 @@
         <v>39</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -688,7 +687,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f t="shared" ref="A5:A40" si="4">A4+1</f>
+        <f t="shared" ref="A5:A38" si="4">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -2120,7 +2119,7 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C40">
         <f>FLOOR(172289.55, 1)</f>
@@ -2129,7 +2128,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C41">
         <f>AVERAGE(C3:C38)</f>
@@ -2138,7 +2137,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3">
         <f>MAX(G3:G38)</f>
@@ -2147,10 +2146,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C43">
-        <f>MAX(K3:K38)</f>
+        <f>MAX(E3:E38)</f>
         <v>5621.0000000000009</v>
       </c>
     </row>

</xml_diff>